<commit_message>
Añadidas descripciones y agregadas en un solo archivo
Aún faltan algunas de VertebradosIbericos que Ale subirá dentro de poco, pero el código para integrarlas está hecho.
</commit_message>
<xml_diff>
--- a/Datos/Datos VertebradosIbericos/Descripciones Anfibios.xlsx
+++ b/Datos/Datos VertebradosIbericos/Descripciones Anfibios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Hackathon\Hackathon-PNAV\Datos\Datos VertebradosIbericos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793FFDA7-C1EE-4C2A-9C1D-65F74C026862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF558C23-DECE-45DE-AC88-35B2E8263493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,16 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
-  <si>
-    <t>Commun Name</t>
-  </si>
-  <si>
-    <t>Scientific Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
   <si>
     <t>Salamandra rabilarga</t>
   </si>
@@ -310,10 +301,25 @@
     <t>Rana de tamaño mediano, de hasta 110 mm de longitud. La coloración es muy variable, aunque suele ser verde, con manchas negras. Usualmente presenta una línea vertebral clara. El tímpano es muy conspicuo y los pliegues dorsolaterales están moderadamente desarrollados. Los dedos de las extremidades posteriores están unidos por membranas interdigitales ampliamente desarrolladas.</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>VertebradosIbericos - Anfibios</t>
+  </si>
+  <si>
+    <t>Nombres comunes</t>
+  </si>
+  <si>
+    <t>Nombre aceptado</t>
+  </si>
+  <si>
+    <t>Fuente</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Grupo taxonómico</t>
+  </si>
+  <si>
+    <t>Anfibios</t>
   </si>
 </sst>
 </file>
@@ -598,460 +604,554 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C24" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C29" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C31" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>